<commit_message>
Publicación desde Crono Pad
</commit_message>
<xml_diff>
--- a/Traducciones/Artículos.xlsx
+++ b/Traducciones/Artículos.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="146">
   <si>
     <t>Data Warehouse Insurance</t>
   </si>
@@ -488,7 +489,7 @@
       <name val="Open Sans"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -525,6 +526,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -538,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -551,6 +564,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -905,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1168,7 +1184,7 @@
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="1">
+      <c r="B21" s="12">
         <v>38421</v>
       </c>
       <c r="C21" t="s">
@@ -1180,7 +1196,7 @@
       </c>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="1">
+      <c r="B22" s="12">
         <v>38687</v>
       </c>
       <c r="C22" t="s">
@@ -1192,7 +1208,7 @@
       </c>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="1">
+      <c r="B23" s="12">
         <v>38869</v>
       </c>
       <c r="C23" t="s">
@@ -1204,7 +1220,7 @@
       </c>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="1">
+      <c r="B24" s="12">
         <v>38904</v>
       </c>
       <c r="C24" t="s">
@@ -1216,7 +1232,7 @@
       </c>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="1">
+      <c r="B25" s="12">
         <v>39293</v>
       </c>
       <c r="C25" t="s">
@@ -1228,7 +1244,7 @@
       </c>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="1">
+      <c r="B26" s="12">
         <v>39358</v>
       </c>
       <c r="C26" t="s">
@@ -1240,7 +1256,7 @@
       </c>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="1">
+      <c r="B27" s="12">
         <v>39375</v>
       </c>
       <c r="C27" t="s">
@@ -1252,7 +1268,7 @@
       </c>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="1">
+      <c r="B28" s="12">
         <v>39376</v>
       </c>
       <c r="C28" t="s">
@@ -1264,7 +1280,7 @@
       </c>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="1">
+      <c r="B29" s="12">
         <v>39427</v>
       </c>
       <c r="C29" t="s">
@@ -1276,7 +1292,7 @@
       </c>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="1">
+      <c r="B30" s="12">
         <v>39681</v>
       </c>
       <c r="C30" t="s">
@@ -1288,7 +1304,7 @@
       </c>
     </row>
     <row r="31" spans="2:5">
-      <c r="B31" s="1">
+      <c r="B31" s="10">
         <v>39694</v>
       </c>
       <c r="C31" t="s">
@@ -1300,7 +1316,7 @@
       </c>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="1">
+      <c r="B32" s="11">
         <v>39714</v>
       </c>
       <c r="C32" t="s">
@@ -1312,7 +1328,7 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="B33" s="1">
+      <c r="B33" s="10">
         <v>39757</v>
       </c>
       <c r="C33" t="s">
@@ -1339,7 +1355,7 @@
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="B35" s="1">
+      <c r="B35" s="10">
         <v>39876</v>
       </c>
       <c r="C35" t="s">
@@ -1366,7 +1382,7 @@
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="B37" s="1">
+      <c r="B37" s="10">
         <v>39967</v>
       </c>
       <c r="C37" t="s">
@@ -1410,7 +1426,7 @@
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="B40" s="1">
+      <c r="B40" s="10">
         <v>40211</v>
       </c>
       <c r="C40" t="s">
@@ -1422,7 +1438,7 @@
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="B41" s="1">
+      <c r="B41" s="10">
         <v>40422</v>
       </c>
       <c r="C41" t="s">
@@ -1434,7 +1450,7 @@
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="B42" s="1">
+      <c r="B42" s="10">
         <v>40434</v>
       </c>
       <c r="C42" t="s">
@@ -1446,7 +1462,7 @@
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="B43" s="1">
+      <c r="B43" s="10">
         <v>40457</v>
       </c>
       <c r="C43" t="s">
@@ -1458,7 +1474,7 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="B44" s="1">
+      <c r="B44" s="10">
         <v>40513</v>
       </c>
       <c r="C44" t="s">
@@ -1470,7 +1486,7 @@
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="B45" s="1">
+      <c r="B45" s="10">
         <v>40638</v>
       </c>
       <c r="C45" t="s">
@@ -1856,4 +1872,102 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="62.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:3">
+      <c r="B5" s="10">
+        <v>39694</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="10">
+        <v>39757</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="10">
+        <v>39876</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="10">
+        <v>39967</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="10">
+        <v>40211</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" s="10">
+        <v>40422</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" s="10">
+        <v>40434</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" s="10">
+        <v>40457</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" s="10">
+        <v>40513</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" s="10">
+        <v>40638</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>